<commit_message>
added the file for create table
</commit_message>
<xml_diff>
--- a/project_report.xlsx
+++ b/project_report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
   <si>
     <t>Project Name</t>
   </si>
@@ -51,19 +51,169 @@
     <t>Budget Variance</t>
   </si>
   <si>
-    <t>creating the solar roof top</t>
-  </si>
-  <si>
-    <t>Planned</t>
+    <t>solar installation</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
   <si>
     <t>200000.00</t>
   </si>
   <si>
-    <t>25412.00</t>
-  </si>
-  <si>
-    <t>-174588.00</t>
+    <t>33134.00</t>
+  </si>
+  <si>
+    <t>200.00000000</t>
+  </si>
+  <si>
+    <t>92507.00</t>
+  </si>
+  <si>
+    <t>92707.00000000</t>
+  </si>
+  <si>
+    <t>-107293.00000000</t>
+  </si>
+  <si>
+    <t>Task ID</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Parent Task</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Planned Start</t>
+  </si>
+  <si>
+    <t>Planned End</t>
+  </si>
+  <si>
+    <t>Actual Start</t>
+  </si>
+  <si>
+    <t>Actual End</t>
+  </si>
+  <si>
+    <t>Estimated Days</t>
+  </si>
+  <si>
+    <t>Estimated Cost</t>
+  </si>
+  <si>
+    <t>Material Cost</t>
+  </si>
+  <si>
+    <t>Labor Cost</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Cost Variance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">design </t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Main Task</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Weekly</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>1500.00</t>
+  </si>
+  <si>
+    <t>6000.00</t>
+  </si>
+  <si>
+    <t>25634.00</t>
+  </si>
+  <si>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t>0E-8</t>
+  </si>
+  <si>
+    <t>-1300.00000000</t>
+  </si>
+  <si>
+    <t>-6000.00000000</t>
+  </si>
+  <si>
+    <t>-25634.00000000</t>
+  </si>
+  <si>
+    <t>Worker Name</t>
+  </si>
+  <si>
+    <t>Specialization</t>
+  </si>
+  <si>
+    <t>Daily Wage</t>
+  </si>
+  <si>
+    <t>Assignment Date</t>
+  </si>
+  <si>
+    <t>Hours Worked</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>praveen</t>
+  </si>
+  <si>
+    <t>material provider</t>
+  </si>
+  <si>
+    <t>800.00</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>Material Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Date Used</t>
+  </si>
+  <si>
+    <t>cement</t>
+  </si>
+  <si>
+    <t>10.00</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>25000.00</t>
   </si>
   <si>
     <t>Date</t>
@@ -81,19 +231,34 @@
     <t>Added By</t>
   </si>
   <si>
-    <t>abc</t>
-  </si>
-  <si>
-    <t>Utilities</t>
-  </si>
-  <si>
-    <t>mret</t>
+    <t>Amount paid to Sridhar N S</t>
+  </si>
+  <si>
+    <t>Amount paid for Electrical Equipments</t>
+  </si>
+  <si>
+    <t>Amount paid to Technical Notification</t>
+  </si>
+  <si>
+    <t>Permits</t>
+  </si>
+  <si>
+    <t>Materials</t>
+  </si>
+  <si>
+    <t>65892.00</t>
+  </si>
+  <si>
+    <t>25413.00</t>
+  </si>
+  <si>
+    <t>1202.00</t>
+  </si>
+  <si>
+    <t>prashanth</t>
   </si>
   <si>
     <t>Cost Type</t>
-  </si>
-  <si>
-    <t>Materials</t>
   </si>
   <si>
     <t>Labor</t>
@@ -507,10 +672,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>45866</v>
+        <v>45860</v>
       </c>
       <c r="C2" s="2">
-        <v>45896</v>
+        <v>45925</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -518,20 +683,20 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -541,43 +706,335 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45859</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45859</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2">
+        <v>45859</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45859</v>
+      </c>
+      <c r="G3" s="2">
+        <v>45866</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="2">
+        <v>45859</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" t="s">
+        <v>42</v>
+      </c>
+      <c r="O3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45923</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45930</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45923</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+      <c r="O4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45859</v>
+      </c>
+      <c r="G2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="2">
+        <v>45860</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -585,36 +1042,70 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>45978</v>
+        <v>45923</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>22</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2">
+        <v>45923</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2">
+        <v>45923</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -632,42 +1123,42 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>80</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated file for task and expenditure of project management
</commit_message>
<xml_diff>
--- a/project_report.xlsx
+++ b/project_report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="93">
   <si>
     <t>Project Name</t>
   </si>
@@ -51,112 +51,148 @@
     <t>Budget Variance</t>
   </si>
   <si>
-    <t>solar installation</t>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>2300000.00</t>
+  </si>
+  <si>
+    <t>38200.00</t>
+  </si>
+  <si>
+    <t>2550.00000000</t>
+  </si>
+  <si>
+    <t>2541.00</t>
+  </si>
+  <si>
+    <t>5091.00000000</t>
+  </si>
+  <si>
+    <t>-2294909.00000000</t>
+  </si>
+  <si>
+    <t>Task ID</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Parent Task</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Planned Start</t>
+  </si>
+  <si>
+    <t>Planned End</t>
+  </si>
+  <si>
+    <t>Actual Start</t>
+  </si>
+  <si>
+    <t>Actual End</t>
+  </si>
+  <si>
+    <t>Estimated Days</t>
+  </si>
+  <si>
+    <t>Estimated Cost</t>
+  </si>
+  <si>
+    <t>Material Cost</t>
+  </si>
+  <si>
+    <t>Labor Cost</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Cost Variance</t>
+  </si>
+  <si>
+    <t>clean land grasses</t>
+  </si>
+  <si>
+    <t>bacement fix</t>
+  </si>
+  <si>
+    <t>dig the land</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>xyz</t>
+  </si>
+  <si>
+    <t>Main Task</t>
+  </si>
+  <si>
+    <t>Daily</t>
   </si>
   <si>
     <t>Completed</t>
   </si>
   <si>
-    <t>200000.00</t>
-  </si>
-  <si>
-    <t>33134.00</t>
-  </si>
-  <si>
-    <t>200.00000000</t>
-  </si>
-  <si>
-    <t>92507.00</t>
-  </si>
-  <si>
-    <t>92707.00000000</t>
-  </si>
-  <si>
-    <t>-107293.00000000</t>
-  </si>
-  <si>
-    <t>Task ID</t>
-  </si>
-  <si>
-    <t>Task Name</t>
-  </si>
-  <si>
-    <t>Parent Task</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Planned Start</t>
-  </si>
-  <si>
-    <t>Planned End</t>
-  </si>
-  <si>
-    <t>Actual Start</t>
-  </si>
-  <si>
-    <t>Actual End</t>
-  </si>
-  <si>
-    <t>Estimated Days</t>
-  </si>
-  <si>
-    <t>Estimated Cost</t>
-  </si>
-  <si>
-    <t>Material Cost</t>
-  </si>
-  <si>
-    <t>Labor Cost</t>
-  </si>
-  <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
-    <t>Cost Variance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">design </t>
-  </si>
-  <si>
-    <t>xyz</t>
-  </si>
-  <si>
-    <t>Main Task</t>
-  </si>
-  <si>
-    <t>Daily</t>
-  </si>
-  <si>
-    <t>Weekly</t>
-  </si>
-  <si>
     <t>Not started</t>
   </si>
   <si>
-    <t>1500.00</t>
-  </si>
-  <si>
-    <t>6000.00</t>
-  </si>
-  <si>
-    <t>25634.00</t>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>3500.00</t>
+  </si>
+  <si>
+    <t>8000.00</t>
+  </si>
+  <si>
+    <t>1100.00</t>
+  </si>
+  <si>
+    <t>2500.00</t>
+  </si>
+  <si>
+    <t>23100.00</t>
   </si>
   <si>
     <t>0.00</t>
   </si>
   <si>
+    <t>1300.00000000</t>
+  </si>
+  <si>
+    <t>500.00000000</t>
+  </si>
+  <si>
+    <t>150.00000000</t>
+  </si>
+  <si>
     <t>0E-8</t>
   </si>
   <si>
-    <t>-1300.00000000</t>
-  </si>
-  <si>
-    <t>-6000.00000000</t>
-  </si>
-  <si>
-    <t>-25634.00000000</t>
+    <t>600.00000000</t>
+  </si>
+  <si>
+    <t>-2200.00000000</t>
+  </si>
+  <si>
+    <t>-7500.00000000</t>
+  </si>
+  <si>
+    <t>-950.00000000</t>
+  </si>
+  <si>
+    <t>-2500.00000000</t>
+  </si>
+  <si>
+    <t>-22500.00000000</t>
   </si>
   <si>
     <t>Worker Name</t>
@@ -186,7 +222,19 @@
     <t>800.00</t>
   </si>
   <si>
-    <t>2.00</t>
+    <t>5.00</t>
+  </si>
+  <si>
+    <t>8.00</t>
+  </si>
+  <si>
+    <t>1.50</t>
+  </si>
+  <si>
+    <t>6.00</t>
+  </si>
+  <si>
+    <t>800.00000000</t>
   </si>
   <si>
     <t>Material Name</t>
@@ -207,7 +255,7 @@
     <t>cement</t>
   </si>
   <si>
-    <t>10.00</t>
+    <t>1.00</t>
   </si>
   <si>
     <t>500</t>
@@ -231,28 +279,10 @@
     <t>Added By</t>
   </si>
   <si>
-    <t>Amount paid to Sridhar N S</t>
-  </si>
-  <si>
-    <t>Amount paid for Electrical Equipments</t>
-  </si>
-  <si>
-    <t>Amount paid to Technical Notification</t>
-  </si>
-  <si>
-    <t>Permits</t>
+    <t>Food</t>
   </si>
   <si>
     <t>Materials</t>
-  </si>
-  <si>
-    <t>65892.00</t>
-  </si>
-  <si>
-    <t>25413.00</t>
-  </si>
-  <si>
-    <t>1202.00</t>
   </si>
   <si>
     <t>prashanth</t>
@@ -672,10 +702,10 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>45860</v>
+        <v>45792</v>
       </c>
       <c r="C2" s="2">
-        <v>45925</v>
+        <v>45980</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -706,7 +736,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -761,143 +791,237 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="F2" s="2">
-        <v>45859</v>
+        <v>45853</v>
       </c>
       <c r="G2" s="2">
-        <v>45859</v>
+        <v>45853</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I2" s="2">
-        <v>45859</v>
+        <v>45855</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="L2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="M2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="N2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="F3" s="2">
-        <v>45859</v>
+        <v>45855</v>
       </c>
       <c r="G3" s="2">
-        <v>45866</v>
+        <v>45856</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" s="2">
-        <v>45859</v>
+        <v>40</v>
+      </c>
+      <c r="I3" t="s">
+        <v>41</v>
       </c>
       <c r="J3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="N3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="O3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45855</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45855</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45855</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" t="s">
+        <v>50</v>
+      </c>
+      <c r="N4" t="s">
+        <v>50</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45923</v>
-      </c>
-      <c r="G4" s="2">
-        <v>45930</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="D5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45856</v>
+      </c>
+      <c r="G5" s="2">
+        <v>45858</v>
+      </c>
+      <c r="H5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="2">
+        <v>45859</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="2">
-        <v>45923</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="D6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45857</v>
+      </c>
+      <c r="G6" s="2">
+        <v>45863</v>
+      </c>
+      <c r="H6" t="s">
         <v>40</v>
       </c>
-      <c r="L4" t="s">
-        <v>41</v>
-      </c>
-      <c r="M4" t="s">
-        <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" t="s">
-        <v>45</v>
+      <c r="I6" s="2">
+        <v>45859</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" t="s">
+        <v>52</v>
+      </c>
+      <c r="O6" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -907,7 +1031,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -921,48 +1045,152 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
       <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45852</v>
+      </c>
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45853</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45855</v>
+      </c>
+      <c r="G4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45855</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45856</v>
+      </c>
+      <c r="G6" t="s">
+        <v>70</v>
+      </c>
+      <c r="H6" t="s">
         <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="2">
-        <v>45859</v>
-      </c>
-      <c r="G2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -986,45 +1214,45 @@
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="H2" s="2">
-        <v>45860</v>
+        <v>45855</v>
       </c>
     </row>
   </sheetData>
@@ -1034,7 +1262,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1042,70 +1270,36 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
-        <v>45923</v>
+        <v>45792</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2">
-        <v>45923</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2">
-        <v>45923</v>
-      </c>
-      <c r="B4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1123,23 +1317,23 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -1147,7 +1341,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -1155,7 +1349,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>

</xml_diff>